<commit_message>
Fix: Remove secondary Y-axis, enable both slider ends, fix UUID reset error
</commit_message>
<xml_diff>
--- a/0. Dati Iniziali/PortfolioMP_Vendite.xlsx
+++ b/0. Dati Iniziali/PortfolioMP_Vendite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PerixMonitor\0. Dati Iniziali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F8DFC3-2717-47D8-9F5A-61580B30CCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9906B2D9-1632-4CF8-9DD9-F94591340C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="5120" windowWidth="26800" windowHeight="10340" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
+    <workbookView xWindow="-110" yWindow="490" windowWidth="38620" windowHeight="21220" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -251,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -278,21 +278,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -309,41 +321,6 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -668,21 +645,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04F4BF02-F5A0-427F-92C4-A60283CF04F1}" name="Table1" displayName="Table1" ref="A1:I5" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04F4BF02-F5A0-427F-92C4-A60283CF04F1}" name="Table1" displayName="Table1" ref="A1:I5" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
   <autoFilter ref="A1:I5" xr:uid="{04F4BF02-F5A0-427F-92C4-A60283CF04F1}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I5">
     <sortCondition ref="F1:F5"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B8061C36-8993-4203-ABD6-C7BF7558D40C}" name="Descrizione Titolo" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{C4CDF0AD-2602-44A7-AA26-292542A274A0}" name="ISIN" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{0A18EC50-C250-41F4-83C1-E84B3FDD76A5}" name="Quantità" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{F21CA34D-52E3-4C7A-A959-24C01F694687}" name="Divisa" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{5C9AD5B2-888B-43C8-AC2C-1789ADAB0AD8}" name="Prezzo Carico (EUR)" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{1CC3BD49-EF04-4684-84DC-5AB42F08A1CD}" name="Data (acquisto/vendita)" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{0B72A75D-196B-42C0-9E49-163198DF8CDB}" name="Operazione" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{8C52C664-8EA8-4E89-892F-C9CCC6BB2E54}" name="Prezzo Operazione (EUR)" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{20AB3F10-3CEF-4BB7-ACA8-F58F613D5EBF}" name="Prezzo Corrente (EUR)" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{B8061C36-8993-4203-ABD6-C7BF7558D40C}" name="Descrizione Titolo" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{C4CDF0AD-2602-44A7-AA26-292542A274A0}" name="ISIN" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{0A18EC50-C250-41F4-83C1-E84B3FDD76A5}" name="Quantità" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{F21CA34D-52E3-4C7A-A959-24C01F694687}" name="Divisa" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{5C9AD5B2-888B-43C8-AC2C-1789ADAB0AD8}" name="Prezzo Carico (EUR)" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{1CC3BD49-EF04-4684-84DC-5AB42F08A1CD}" name="Data (acquisto/vendita)" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{0B72A75D-196B-42C0-9E49-163198DF8CDB}" name="Operazione" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{8C52C664-8EA8-4E89-892F-C9CCC6BB2E54}" name="Prezzo Operazione (EUR)" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{20AB3F10-3CEF-4BB7-ACA8-F58F613D5EBF}" name="Prezzo Corrente (EUR)" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1008,7 +985,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1124,18 +1101,18 @@
       <c r="I4" s="11"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="7">
         <v>3198</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="15">
+      <c r="D5" s="8"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="9">
         <v>46038</v>
       </c>
       <c r="G5" s="10" t="s">
@@ -1145,39 +1122,39 @@
         <f>16162.69/Table1[[#This Row],[Quantità]]</f>
         <v>5.0539993746091305</v>
       </c>
-      <c r="I5" s="16"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H10" s="17"/>
+      <c r="H10" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A5">
-    <cfRule type="containsText" dxfId="8" priority="18" stopIfTrue="1" operator="containsText" text="BTP">
+    <cfRule type="containsText" dxfId="6" priority="18" stopIfTrue="1" operator="containsText" text="BTP">
       <formula>NOT(ISERROR(SEARCH("BTP",A2)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="19" stopIfTrue="1">
       <formula>IF(AND(ISNUMBER(SEARCH("H2O", A2)), ISNUMBER(SEARCH("SP", A2))), 1,0)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="containsText" dxfId="4" priority="1" stopIfTrue="1" operator="containsText" text="BTP">
+      <formula>NOT(ISERROR(SEARCH("BTP",A5)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
+      <formula>IF(AND(ISNUMBER(SEARCH("H2O", A5)), ISNUMBER(SEARCH("SP", A5))), 1,0)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C2:C4">
-    <cfRule type="containsBlanks" dxfId="6" priority="16">
+    <cfRule type="containsBlanks" dxfId="2" priority="16">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G5">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Vendita">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Vendita">
       <formula>NOT(ISERROR(SEARCH("Vendita",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Acquisto">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Acquisto">
       <formula>NOT(ISERROR(SEARCH("Acquisto",G2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5">
-    <cfRule type="containsText" dxfId="1" priority="1" stopIfTrue="1" operator="containsText" text="BTP">
-      <formula>NOT(ISERROR(SEARCH("BTP",A5)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
-      <formula>IF(AND(ISNUMBER(SEARCH("H2O", A5)), ISNUMBER(SEARCH("SP", A5))), 1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>